<commit_message>
Auto increment in Roll No. added
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\DataTableActivity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7379CA5-03A8-4BF1-900F-E30308BF8823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56146B95-469C-41E7-9A92-41FA481B6076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -734,130 +734,180 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D8AD9C-782B-4546-ACFA-34A7BDC0D66E}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="A1:C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
         <v>14.6666666666667</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5">
         <v>3.6666666666666701</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6">
         <v>16.6666666666667</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
       <c r="B7">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8">
         <v>19.3333333333333</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9">
         <v>13.3333333333333</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11">
         <v>16.6666666666667</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12">
         <v>15.3333333333333</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13">
         <v>16.6666666666667</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
       <c r="B14">
         <v>16.6666666666667</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15">
         <v>14.3333333333333</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove Data Column Activity
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\DataTableActivity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56146B95-469C-41E7-9A92-41FA481B6076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F0A413-9F2A-4ECB-B1CA-23A9EC8172E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -734,10 +734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D8AD9C-782B-4546-ACFA-34A7BDC0D66E}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="A1:C15"/>
+      <selection activeCell="I17" sqref="E1:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -755,8 +755,14 @@
       <c r="C1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -766,8 +772,14 @@
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -777,8 +789,14 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -788,8 +806,14 @@
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -799,8 +823,14 @@
       <c r="C5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -810,8 +840,14 @@
       <c r="C6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -821,8 +857,14 @@
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -832,8 +874,14 @@
       <c r="C8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -843,8 +891,14 @@
       <c r="C9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -854,8 +908,14 @@
       <c r="C10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -865,8 +925,14 @@
       <c r="C11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -876,8 +942,14 @@
       <c r="C12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -887,8 +959,14 @@
       <c r="C13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -898,8 +976,14 @@
       <c r="C14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -907,6 +991,12 @@
         <v>14.3333333333333</v>
       </c>
       <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove Data Row Activity
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\DataTableActivity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F0A413-9F2A-4ECB-B1CA-23A9EC8172E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36610172-84F8-474E-9FA5-4A698FC77756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -736,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D8AD9C-782B-4546-ACFA-34A7BDC0D66E}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="E1:I17"/>
     </sheetView>
   </sheetViews>
@@ -1006,6 +1007,343 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6FD2F5-E527-44EA-A8E3-614AEAFC9BBC}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1011</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1018</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>14.666666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1015</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1020</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1022</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1010</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>19.333333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1019</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1016</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1012</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1013</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>19</v>
+      </c>
+      <c r="G11">
+        <v>15.333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1014</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1023</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>18</v>
+      </c>
+      <c r="G13">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1017</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>15</v>
+      </c>
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>18</v>
+      </c>
+      <c r="G14">
+        <v>14.333333333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>

</xml_diff>

<commit_message>
Remove Data Row Activities
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\DataTableActivity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36610172-84F8-474E-9FA5-4A698FC77756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A89C15-B179-4D29-93B4-F28F9290B462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -724,7 +724,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="A1:G17"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,10 +735,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D8AD9C-782B-4546-ACFA-34A7BDC0D66E}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="E1:I17"/>
+      <selection activeCell="H15" sqref="E1:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +746,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -756,14 +756,8 @@
       <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -773,14 +767,8 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -790,14 +778,8 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -807,14 +789,8 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -824,14 +800,8 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -841,14 +811,8 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -858,14 +822,8 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -875,14 +833,8 @@
       <c r="C8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -892,14 +844,8 @@
       <c r="C9">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -909,14 +855,8 @@
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -926,14 +866,8 @@
       <c r="C11">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -943,14 +877,8 @@
       <c r="C12">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -960,14 +888,8 @@
       <c r="C13">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -977,14 +899,8 @@
       <c r="C14">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -992,12 +908,6 @@
         <v>14.3333333333333</v>
       </c>
       <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15">
         <v>13</v>
       </c>
     </row>
@@ -1008,10 +918,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6FD2F5-E527-44EA-A8E3-614AEAFC9BBC}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="G15" sqref="A1:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,13 +1181,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1014</v>
+        <v>1023</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <v>17</v>
@@ -1294,25 +1204,25 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1023</v>
+        <v>1017</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D13">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>18</v>
       </c>
       <c r="G13">
-        <v>16.666666666666668</v>
+        <v>14.333333333333334</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1335,6 +1245,29 @@
         <v>18</v>
       </c>
       <c r="G14">
+        <v>14.333333333333334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1017</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>18</v>
+      </c>
+      <c r="G15">
         <v>14.333333333333334</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove Duplicate Rows Acitivity
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\DataTableActivity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065F30C6-47F0-48E5-A6B4-48DFFD58C128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43001A3B-F3FA-421C-8B66-2919DCFFF038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Duplicates Removed" sheetId="9" r:id="rId5"/>
+    <sheet name="Duplicates" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -185,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,6 +201,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -920,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6FD2F5-E527-44EA-A8E3-614AEAFC9BBC}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
@@ -1232,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,118 +1637,118 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D18" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" ref="G18:G31" si="1">SUM(D18:F18)/3</f>
-        <v>18</v>
+        <f t="shared" ref="G18:G33" si="1">SUM(D18:F18)/3</f>
+        <v>19.333333333333332</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>1018</v>
+        <v>1011</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E19" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F19" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G19" s="4">
         <f t="shared" si="1"/>
-        <v>14.666666666666666</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D20" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E20" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F20" s="4">
         <v>18</v>
       </c>
       <c r="G20" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>16.666666666666668</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>1020</v>
+        <v>1013</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D21" s="4">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E21" s="4">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F21" s="4">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="1"/>
-        <v>3.6666666666666665</v>
+        <v>15.333333333333334</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>1022</v>
+        <v>1014</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D22" s="4">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E22" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F22" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G22" s="4">
         <f t="shared" si="1"/>
@@ -1754,190 +1757,190 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>1021</v>
+        <v>1015</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D23" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E23" s="4">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F23" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G23" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D24" s="4">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E24" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G24" s="4">
         <f t="shared" si="1"/>
-        <v>19.333333333333332</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D25" s="4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E25" s="4">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F25" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G25" s="4">
         <f t="shared" si="1"/>
-        <v>13.333333333333334</v>
+        <v>14.333333333333334</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D26" s="4">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E26" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F26" s="4">
         <v>19</v>
       </c>
       <c r="G26" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>14.666666666666666</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>1012</v>
+        <v>1019</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="4">
+        <v>12</v>
+      </c>
+      <c r="E27" s="4">
         <v>13</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="4">
-        <v>15</v>
-      </c>
-      <c r="E27" s="4">
-        <v>17</v>
-      </c>
       <c r="F27" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G27" s="4">
         <f t="shared" si="1"/>
-        <v>16.666666666666668</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>1013</v>
+        <v>1020</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D28" s="4">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E28" s="4">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F28" s="4">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="G28" s="4">
         <f t="shared" si="1"/>
-        <v>15.333333333333334</v>
+        <v>3.6666666666666665</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>1014</v>
+        <v>1021</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D29" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E29" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F29" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G29" s="4">
         <f t="shared" si="1"/>
-        <v>16.666666666666668</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D30" s="4">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E30" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F30" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G30" s="4">
         <f t="shared" si="1"/>
@@ -1946,33 +1949,845 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>1017</v>
+        <v>1023</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D31" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E31" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F31" s="4">
         <v>18</v>
       </c>
       <c r="G31" s="4">
         <f t="shared" si="1"/>
-        <v>14.333333333333334</v>
-      </c>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:G31">
+    <sortCondition ref="A18:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625C4A41-862A-490A-B69D-9A015E2C6A68}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1010</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7">
+        <v>19</v>
+      </c>
+      <c r="E2" s="7">
+        <v>19</v>
+      </c>
+      <c r="F2" s="7">
+        <v>20</v>
+      </c>
+      <c r="G2" s="7">
+        <v>19.333333333333332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1011</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7">
+        <v>18</v>
+      </c>
+      <c r="G3" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1012</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7">
+        <v>17</v>
+      </c>
+      <c r="F4" s="7">
+        <v>18</v>
+      </c>
+      <c r="G4" s="7">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1013</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7">
+        <v>15.333333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1014</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7">
+        <v>15</v>
+      </c>
+      <c r="F6" s="7">
+        <v>18</v>
+      </c>
+      <c r="G6" s="7">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1015</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="7">
+        <v>18</v>
+      </c>
+      <c r="E7" s="7">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7">
+        <v>18</v>
+      </c>
+      <c r="G7" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1016</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7">
+        <v>18</v>
+      </c>
+      <c r="F8" s="7">
+        <v>19</v>
+      </c>
+      <c r="G8" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1017</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7">
+        <v>18</v>
+      </c>
+      <c r="G9" s="7">
+        <v>14.333333333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1018</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="7">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7">
+        <v>15</v>
+      </c>
+      <c r="F10" s="7">
+        <v>19</v>
+      </c>
+      <c r="G10" s="7">
+        <v>14.666666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1019</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="7">
+        <v>12</v>
+      </c>
+      <c r="E11" s="7">
+        <v>13</v>
+      </c>
+      <c r="F11" s="7">
+        <v>15</v>
+      </c>
+      <c r="G11" s="7">
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1020</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>4</v>
+      </c>
+      <c r="G12" s="7">
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1021</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7">
+        <v>19</v>
+      </c>
+      <c r="F13" s="7">
+        <v>20</v>
+      </c>
+      <c r="G13" s="7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1022</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="7">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7">
+        <v>18</v>
+      </c>
+      <c r="F14" s="7">
+        <v>20</v>
+      </c>
+      <c r="G14" s="7">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1023</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="7">
+        <v>17</v>
+      </c>
+      <c r="E15" s="7">
+        <v>15</v>
+      </c>
+      <c r="F15" s="7">
+        <v>18</v>
+      </c>
+      <c r="G15" s="7">
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="7">
+        <v>18</v>
+      </c>
+      <c r="E16" s="7">
+        <v>15</v>
+      </c>
+      <c r="F16" s="7">
+        <v>18</v>
+      </c>
+      <c r="G16" s="7">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC06DB00-5124-4138-BF72-3C537F34C12C}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1010</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4">
+        <v>20</v>
+      </c>
+      <c r="G2" s="4">
+        <f t="shared" ref="G2:G17" si="0">SUM(D2:F2)/3</f>
+        <v>19.333333333333332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1011</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1012</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1013</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>15.333333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1014</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4">
+        <v>15</v>
+      </c>
+      <c r="F6" s="4">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>1015</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>18</v>
+      </c>
+      <c r="E7" s="4">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1016</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4">
+        <v>19</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>1017</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4">
+        <v>18</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>14.333333333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1018</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4">
+        <v>19</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>14.666666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1019</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12</v>
+      </c>
+      <c r="E11" s="4">
+        <v>13</v>
+      </c>
+      <c r="F11" s="4">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1020</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>4</v>
+      </c>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1021</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="4">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1022</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="4">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4">
+        <v>20</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1023</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="4">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4">
+        <v>18</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1024</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="4">
+        <v>18</v>
+      </c>
+      <c r="E16" s="4">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4">
+        <v>18</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>